<commit_message>
Add magic dogs to content lists
</commit_message>
<xml_diff>
--- a/PublicContentList.xlsx
+++ b/PublicContentList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\D&amp;D\Homebrew\DnD-Homebrew\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D726F4F9-9865-45F1-8AEF-54DDD1B01ECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44276390-EC4F-4FF2-B3D7-171CD5EE6B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Creatures" sheetId="1" r:id="rId1"/>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2770" uniqueCount="575">
   <si>
     <t>Name</t>
   </si>
@@ -1917,6 +1917,36 @@
   </si>
   <si>
     <t>Magic Chariots</t>
+  </si>
+  <si>
+    <t>Aralez</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Extraplanar, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Urban</t>
+  </si>
+  <si>
+    <t>Chamrosh</t>
+  </si>
+  <si>
+    <t>Coastal, Desert, Extraplanar, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp,</t>
+  </si>
+  <si>
+    <t>Flood Hound</t>
+  </si>
+  <si>
+    <t>Elemental</t>
+  </si>
+  <si>
+    <t>Arctic, Coastal, Desert, Extraplanar, Forest, Freshwater, Grassland, Hills, Jungle, Mountain, Swamp, Underwater, Urban</t>
+  </si>
+  <si>
+    <t>Miniature Blink Dog</t>
+  </si>
+  <si>
+    <t>Extraplanar, Forest, Grassland, Hills</t>
+  </si>
+  <si>
+    <t>Magic Dogs</t>
   </si>
 </sst>
 </file>
@@ -2242,6 +2272,24 @@
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2258,24 +2306,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2815,11 +2845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I165"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A166" sqref="A166"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D172" sqref="D172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7620,6 +7650,122 @@
         <v>40</v>
       </c>
       <c r="I165" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C166" s="6">
+        <v>3</v>
+      </c>
+      <c r="D166" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E166" s="37" t="s">
+        <v>566</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="G166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H166" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I166" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A167" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C167" s="6">
+        <v>7</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="E167" s="37" t="s">
+        <v>568</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H167" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I167" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C168" s="6">
+        <v>1</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="E168" s="37" t="s">
+        <v>571</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="G168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H168" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I168" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A169" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C169" s="6">
+        <v>0.125</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E169" s="37" t="s">
+        <v>573</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="G169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H169" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I169" s="1" t="s">
         <v>40</v>
       </c>
     </row>
@@ -7807,9 +7953,11 @@
     <hyperlink ref="F156:F163" r:id="rId94" display="Dogs" xr:uid="{76B9A0A5-62FA-469A-812A-8AB42A7B076F}"/>
     <hyperlink ref="F164" r:id="rId95" xr:uid="{D40EA6A1-C093-496E-859C-C44BF7C9329E}"/>
     <hyperlink ref="F165" r:id="rId96" xr:uid="{A91F655D-D2F4-44F6-9210-7F3A21ADD68A}"/>
+    <hyperlink ref="F166" r:id="rId97" xr:uid="{1B6DB6F3-249D-431B-AFD9-B5A35361723B}"/>
+    <hyperlink ref="F167:F169" r:id="rId98" display="Magic Dogs" xr:uid="{5C4FDEE5-B0A8-4348-8234-1910AE193D72}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId97"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId99"/>
 </worksheet>
 </file>
 
@@ -8001,87 +8149,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="19" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="38" t="s">
         <v>430</v>
       </c>
-      <c r="C1" s="44" t="s">
+      <c r="C1" s="38" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="44" t="s">
+      <c r="D1" s="38" t="s">
         <v>371</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="42" t="s">
         <v>372</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="40" t="s">
         <v>373</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="40" t="s">
         <v>374</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="40" t="s">
         <v>375</v>
       </c>
-      <c r="I1" s="46" t="s">
+      <c r="I1" s="40" t="s">
         <v>376</v>
       </c>
-      <c r="J1" s="38" t="s">
+      <c r="J1" s="44" t="s">
         <v>377</v>
       </c>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
     </row>
     <row r="2" spans="1:15" s="19" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="44"/>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="40" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="46" t="s">
         <v>381</v>
       </c>
-      <c r="K2" s="42" t="s">
+      <c r="K2" s="48" t="s">
         <v>382</v>
       </c>
-      <c r="L2" s="42" t="s">
+      <c r="L2" s="48" t="s">
         <v>383</v>
       </c>
-      <c r="M2" s="42" t="s">
+      <c r="M2" s="48" t="s">
         <v>384</v>
       </c>
-      <c r="N2" s="42" t="s">
+      <c r="N2" s="48" t="s">
         <v>385</v>
       </c>
-      <c r="O2" s="42" t="s">
+      <c r="O2" s="48" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="19" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="43"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="47"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
     </row>
     <row r="4" spans="1:15" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
@@ -8618,6 +8766,13 @@
     </sortState>
   </autoFilter>
   <mergeCells count="16">
+    <mergeCell ref="J1:O1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="C1:C3"/>
     <mergeCell ref="H1:H3"/>
     <mergeCell ref="I1:I3"/>
@@ -8627,13 +8782,6 @@
     <mergeCell ref="E1:E3"/>
     <mergeCell ref="F1:F3"/>
     <mergeCell ref="G1:G3"/>
-    <mergeCell ref="J1:O1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{B4A7D905-D120-4788-AC98-B53455EB3FC4}"/>
@@ -11102,7 +11250,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BDE69A5-0DEA-4E6C-8C42-A4C78FD0BD58}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>

</xml_diff>